<commit_message>
missing part is added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Task_1.xlsx
+++ b/src/test/resources/testData/Task_1.xlsx
@@ -26,12 +26,17 @@
     <sheet name="Optometry_Paymnt" r:id="rId20" sheetId="18"/>
     <sheet name="Optometry_Manufactr" r:id="rId21" sheetId="19"/>
     <sheet name="Optometry_Revenue" r:id="rId22" sheetId="20"/>
+    <sheet name="Chiropractic_BPM" r:id="rId23" sheetId="21"/>
+    <sheet name="Chiropractic_PatMartk" r:id="rId24" sheetId="22"/>
+    <sheet name="Chiropractic_Paymnt" r:id="rId25" sheetId="23"/>
+    <sheet name="Chiropractic_Manufactr" r:id="rId26" sheetId="24"/>
+    <sheet name="Chiropractic_Revenue" r:id="rId27" sheetId="25"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="66">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -45,159 +50,159 @@
     <t>App Name</t>
   </si>
   <si>
+    <t>PatientHomePage</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Business Performance Management</t>
+  </si>
+  <si>
+    <t>MaevaDentalAdvisors</t>
+  </si>
+  <si>
+    <t>chrisad</t>
+  </si>
+  <si>
+    <t>CyberScoutElite</t>
+  </si>
+  <si>
+    <t>SmileSource</t>
+  </si>
+  <si>
+    <t>OrthoPOPremium</t>
+  </si>
+  <si>
+    <t>FeeSurveyforDentistry</t>
+  </si>
+  <si>
+    <t>DentalPOEssentials</t>
+  </si>
+  <si>
+    <t>DentalPOPremium</t>
+  </si>
+  <si>
+    <t>FeeOptimizerforDentistry</t>
+  </si>
+  <si>
+    <t>IndustryTrendsData</t>
+  </si>
+  <si>
     <t>practicemobilizer</t>
   </si>
   <si>
-    <t>Dental</t>
-  </si>
-  <si>
-    <t>Business Performance Management</t>
-  </si>
-  <si>
-    <t>FeeOptimizerforDentistry</t>
-  </si>
-  <si>
-    <t>SmileSource</t>
-  </si>
-  <si>
-    <t>IndustryTrendsData</t>
-  </si>
-  <si>
-    <t>chrisad</t>
-  </si>
-  <si>
-    <t>PatientHomePage</t>
-  </si>
-  <si>
-    <t>FeeSurveyforDentistry</t>
-  </si>
-  <si>
-    <t>CyberScoutElite</t>
-  </si>
-  <si>
-    <t>MaevaDentalAdvisors</t>
-  </si>
-  <si>
-    <t>DentalPOEssentials</t>
-  </si>
-  <si>
-    <t>OrthoPOPremium</t>
-  </si>
-  <si>
-    <t>DentalPOPremium</t>
+    <t>myaffordabledentalmarketing</t>
+  </si>
+  <si>
+    <t>Patient Marketing</t>
+  </si>
+  <si>
+    <t>DentalWebSites</t>
+  </si>
+  <si>
+    <t>TestimonialTree</t>
+  </si>
+  <si>
+    <t>DigitalMarketerMD</t>
+  </si>
+  <si>
+    <t>Swell</t>
+  </si>
+  <si>
+    <t>patientnews</t>
+  </si>
+  <si>
+    <t>connectthedoc</t>
+  </si>
+  <si>
+    <t>Doctible</t>
+  </si>
+  <si>
+    <t>RepuGen</t>
+  </si>
+  <si>
+    <t>SmartMarket</t>
+  </si>
+  <si>
+    <t>PracticeAI</t>
+  </si>
+  <si>
+    <t>RhinogramRegistration</t>
   </si>
   <si>
     <t>BirdEye</t>
   </si>
   <si>
-    <t>Patient Marketing</t>
-  </si>
-  <si>
-    <t>DigitalMarketerMD</t>
-  </si>
-  <si>
-    <t>connectthedoc</t>
-  </si>
-  <si>
-    <t>myaffordabledentalmarketing</t>
-  </si>
-  <si>
-    <t>Doctible</t>
-  </si>
-  <si>
-    <t>DentalWebSites</t>
-  </si>
-  <si>
-    <t>Swell</t>
-  </si>
-  <si>
     <t>PatientPopRegister</t>
   </si>
   <si>
-    <t>PracticeAI</t>
-  </si>
-  <si>
-    <t>RhinogramRegistration</t>
-  </si>
-  <si>
-    <t>SmartMarket</t>
-  </si>
-  <si>
-    <t>patientnews</t>
-  </si>
-  <si>
-    <t>RepuGen</t>
-  </si>
-  <si>
-    <t>TestimonialTree</t>
+    <t>SikkaPayments</t>
+  </si>
+  <si>
+    <t>Payments</t>
   </si>
   <si>
     <t>PartiallyPaymentPlans</t>
   </si>
   <si>
-    <t>Payments</t>
+    <t>kleer</t>
   </si>
   <si>
     <t>Pearly</t>
   </si>
   <si>
-    <t>SikkaPayments</t>
-  </si>
-  <si>
-    <t>kleer</t>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>Manufacturers/Labs</t>
+  </si>
+  <si>
+    <t>AmazonDental</t>
+  </si>
+  <si>
+    <t>Midmark</t>
+  </si>
+  <si>
+    <t>DigitalDentalExchange</t>
+  </si>
+  <si>
+    <t>MicrodentalLaboratories</t>
   </si>
   <si>
     <t>DentsplySirona</t>
   </si>
   <si>
-    <t>Manufacturers/Labs</t>
-  </si>
-  <si>
-    <t>DigitalDentalExchange</t>
+    <t>HP</t>
   </si>
   <si>
     <t>Invisalign</t>
   </si>
   <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>Midmark</t>
-  </si>
-  <si>
-    <t>AmazonDental</t>
-  </si>
-  <si>
-    <t>MicrodentalLaboratories</t>
-  </si>
-  <si>
-    <t>3M</t>
+    <t>ICSystem</t>
+  </si>
+  <si>
+    <t>Revenue Cycle</t>
+  </si>
+  <si>
+    <t>Illumitrac</t>
+  </si>
+  <si>
+    <t>TekCollect</t>
+  </si>
+  <si>
+    <t>SmartCollect</t>
+  </si>
+  <si>
+    <t>MyIntegrations</t>
   </si>
   <si>
     <t>Abellaregistration</t>
   </si>
   <si>
-    <t>Revenue Cycle</t>
-  </si>
-  <si>
-    <t>MyIntegrations</t>
-  </si>
-  <si>
-    <t>SmartCollect</t>
-  </si>
-  <si>
-    <t>TekCollect</t>
-  </si>
-  <si>
-    <t>Illumitrac</t>
-  </si>
-  <si>
     <t>CapitalAccounts</t>
   </si>
   <si>
-    <t>ICSystem</t>
-  </si>
-  <si>
     <t>Veterinary</t>
   </si>
   <si>
@@ -207,25 +212,28 @@
     <t>VeterinaryOCE</t>
   </si>
   <si>
+    <t>VeterinaryPOPremium</t>
+  </si>
+  <si>
     <t>FeeSurveyforVeterinary</t>
   </si>
   <si>
-    <t>VeterinaryPOPremium</t>
-  </si>
-  <si>
     <t>SikkaSwellVetBundle</t>
   </si>
   <si>
+    <t>RoyalCanin</t>
+  </si>
+  <si>
     <t>HillsToHome</t>
   </si>
   <si>
-    <t>RoyalCanin</t>
-  </si>
-  <si>
     <t>Physician</t>
   </si>
   <si>
     <t>Optometry</t>
+  </si>
+  <si>
+    <t>Chiropractic</t>
   </si>
 </sst>
 </file>
@@ -233,13 +241,38 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="21">
+  <fonts count="26">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -372,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -454,6 +487,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -692,7 +745,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s" s="20">
         <v>55</v>
@@ -706,7 +759,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s" s="20">
         <v>55</v>
@@ -720,7 +773,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s" s="20">
         <v>55</v>
@@ -734,7 +787,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s" s="20">
         <v>55</v>
@@ -814,7 +867,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s" s="24">
         <v>63</v>
@@ -828,7 +881,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s" s="24">
         <v>63</v>
@@ -842,7 +895,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s" s="24">
         <v>63</v>
@@ -856,7 +909,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s" s="24">
         <v>63</v>
@@ -903,7 +956,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s" s="26">
         <v>63</v>
@@ -1058,7 +1111,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s" s="32">
         <v>64</v>
@@ -1105,7 +1158,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s" s="34">
         <v>64</v>
@@ -1119,7 +1172,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s" s="34">
         <v>64</v>
@@ -1133,7 +1186,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s" s="34">
         <v>64</v>
@@ -1147,7 +1200,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s" s="34">
         <v>64</v>
@@ -1175,7 +1228,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s" s="34">
         <v>64</v>
@@ -1222,7 +1275,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s" s="36">
         <v>64</v>
@@ -1244,10 +1297,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.4375" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="23.4375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="23.4375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="23.4375" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.4375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1269,7 +1322,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s" s="38">
         <v>64</v>
@@ -1520,6 +1573,381 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
+    <col min="1" max="1" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.4375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="39">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="39">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="39">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="40">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s" s="40">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="40">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s" s="40">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="40">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s" s="40">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="40">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s" s="40">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.4375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="41">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="41">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="41">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="42">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s" s="42">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="42">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="42">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.4375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="43">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="43">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="43">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="44">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s" s="44">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="44">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s" s="44">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="44">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s" s="44">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="44">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s" s="44">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="44">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="44">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="44">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s" s="44">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.4375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.4375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="45">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="45">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="45">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="46">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s" s="46">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="46">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s" s="46">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.4375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="23.4375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="23.4375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="23.4375" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="47">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="47">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="47">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="48">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s" s="48">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
     <col min="1" max="1" width="23.4375" customWidth="true"/>
     <col min="2" max="2" width="23.4375" customWidth="true"/>
     <col min="3" max="3" width="23.4375" customWidth="true"/>
@@ -1527,70 +1955,70 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="39">
+      <c r="A1" t="s" s="49">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="39">
+      <c r="B1" t="s" s="49">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="39">
+      <c r="C1" t="s" s="49">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="39">
+      <c r="D1" t="s" s="49">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="40">
+      <c r="A2" t="n" s="50">
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" t="s" s="40">
-        <v>64</v>
+      <c r="C2" t="s" s="50">
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="40">
+      <c r="A3" t="n" s="50">
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s" s="40">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="C3" t="s" s="50">
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="40">
+      <c r="A4" t="n" s="50">
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s" s="40">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="C4" t="s" s="50">
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="40">
+      <c r="A5" t="n" s="50">
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s" s="40">
-        <v>64</v>
+        <v>50</v>
+      </c>
+      <c r="C5" t="s" s="50">
+        <v>65</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -1999,7 +2427,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s" s="12">
         <v>55</v>
@@ -2027,7 +2455,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s" s="12">
         <v>55</v>
@@ -2041,7 +2469,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s" s="12">
         <v>55</v>
@@ -2055,7 +2483,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s" s="12">
         <v>55</v>
@@ -2069,7 +2497,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s" s="12">
         <v>55</v>
@@ -2083,7 +2511,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s" s="12">
         <v>55</v>
@@ -2130,7 +2558,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s" s="14">
         <v>55</v>
@@ -2158,7 +2586,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s" s="14">
         <v>55</v>
@@ -2172,7 +2600,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s" s="14">
         <v>55</v>
@@ -2186,7 +2614,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s" s="14">
         <v>55</v>
@@ -2200,7 +2628,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s" s="14">
         <v>55</v>
@@ -2261,7 +2689,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s" s="16">
         <v>55</v>
@@ -2308,7 +2736,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s" s="18">
         <v>55</v>
@@ -2322,7 +2750,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s" s="18">
         <v>55</v>
@@ -2336,7 +2764,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s" s="18">
         <v>55</v>

</xml_diff>

<commit_message>
Headless added to setUpMethod
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Task_1.xlsx
+++ b/src/test/resources/testData/Task_1.xlsx
@@ -50,139 +50,148 @@
     <t>App Name</t>
   </si>
   <si>
+    <t>IndustryTrendsData</t>
+  </si>
+  <si>
+    <t>dental</t>
+  </si>
+  <si>
+    <t>business performance management</t>
+  </si>
+  <si>
+    <t>CyberScoutElite</t>
+  </si>
+  <si>
+    <t>chrisad</t>
+  </si>
+  <si>
     <t>PatientHomePage</t>
   </si>
   <si>
-    <t>Dental</t>
-  </si>
-  <si>
-    <t>Business Performance Management</t>
+    <t>FeeSurveyforDentistry</t>
+  </si>
+  <si>
+    <t>OrthoPOPremium</t>
+  </si>
+  <si>
+    <t>FeeOptimizerforDentistry</t>
+  </si>
+  <si>
+    <t>SmileSource</t>
+  </si>
+  <si>
+    <t>practicemobilizer</t>
   </si>
   <si>
     <t>MaevaDentalAdvisors</t>
   </si>
   <si>
-    <t>chrisad</t>
-  </si>
-  <si>
-    <t>CyberScoutElite</t>
-  </si>
-  <si>
-    <t>SmileSource</t>
-  </si>
-  <si>
-    <t>OrthoPOPremium</t>
-  </si>
-  <si>
-    <t>FeeSurveyforDentistry</t>
+    <t>DentalPOPremium</t>
   </si>
   <si>
     <t>DentalPOEssentials</t>
   </si>
   <si>
-    <t>DentalPOPremium</t>
-  </si>
-  <si>
-    <t>FeeOptimizerforDentistry</t>
-  </si>
-  <si>
-    <t>IndustryTrendsData</t>
-  </si>
-  <si>
-    <t>practicemobilizer</t>
+    <t>RhinogramRegistration</t>
+  </si>
+  <si>
+    <t>patient marketing</t>
+  </si>
+  <si>
+    <t>BirdEye</t>
+  </si>
+  <si>
+    <t>patientnews</t>
+  </si>
+  <si>
+    <t>RepuGen</t>
+  </si>
+  <si>
+    <t>PatientPopRegister</t>
+  </si>
+  <si>
+    <t>Doctible</t>
+  </si>
+  <si>
+    <t>connectthedoc</t>
+  </si>
+  <si>
+    <t>DentalWebSites</t>
+  </si>
+  <si>
+    <t>DigitalMarketerMD</t>
+  </si>
+  <si>
+    <t>TestimonialTree</t>
+  </si>
+  <si>
+    <t>PracticeAI</t>
   </si>
   <si>
     <t>myaffordabledentalmarketing</t>
   </si>
   <si>
-    <t>Patient Marketing</t>
-  </si>
-  <si>
-    <t>DentalWebSites</t>
-  </si>
-  <si>
-    <t>TestimonialTree</t>
-  </si>
-  <si>
-    <t>DigitalMarketerMD</t>
-  </si>
-  <si>
     <t>Swell</t>
   </si>
   <si>
-    <t>patientnews</t>
-  </si>
-  <si>
-    <t>connectthedoc</t>
-  </si>
-  <si>
-    <t>Doctible</t>
-  </si>
-  <si>
-    <t>RepuGen</t>
-  </si>
-  <si>
     <t>SmartMarket</t>
   </si>
   <si>
-    <t>PracticeAI</t>
-  </si>
-  <si>
-    <t>RhinogramRegistration</t>
-  </si>
-  <si>
-    <t>BirdEye</t>
-  </si>
-  <si>
-    <t>PatientPopRegister</t>
+    <t>PartiallyPaymentPlans</t>
+  </si>
+  <si>
+    <t>payments</t>
   </si>
   <si>
     <t>SikkaPayments</t>
   </si>
   <si>
-    <t>Payments</t>
-  </si>
-  <si>
-    <t>PartiallyPaymentPlans</t>
+    <t>Pearly</t>
   </si>
   <si>
     <t>kleer</t>
   </si>
   <si>
-    <t>Pearly</t>
+    <t>Invisalign</t>
+  </si>
+  <si>
+    <t>manufacturers/labs</t>
+  </si>
+  <si>
+    <t>Midmark</t>
+  </si>
+  <si>
+    <t>MicrodentalLaboratories</t>
   </si>
   <si>
     <t>3M</t>
   </si>
   <si>
-    <t>Manufacturers/Labs</t>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>DigitalDentalExchange</t>
   </si>
   <si>
     <t>AmazonDental</t>
   </si>
   <si>
-    <t>Midmark</t>
-  </si>
-  <si>
-    <t>DigitalDentalExchange</t>
-  </si>
-  <si>
-    <t>MicrodentalLaboratories</t>
-  </si>
-  <si>
     <t>DentsplySirona</t>
   </si>
   <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>Invisalign</t>
+    <t>CapitalAccounts</t>
+  </si>
+  <si>
+    <t>revenue cycle</t>
   </si>
   <si>
     <t>ICSystem</t>
   </si>
   <si>
-    <t>Revenue Cycle</t>
+    <t>Abellaregistration</t>
+  </si>
+  <si>
+    <t>MyIntegrations</t>
   </si>
   <si>
     <t>Illumitrac</t>
@@ -194,46 +203,37 @@
     <t>SmartCollect</t>
   </si>
   <si>
-    <t>MyIntegrations</t>
-  </si>
-  <si>
-    <t>Abellaregistration</t>
-  </si>
-  <si>
-    <t>CapitalAccounts</t>
-  </si>
-  <si>
-    <t>Veterinary</t>
+    <t>veterinary</t>
+  </si>
+  <si>
+    <t>FeeSurveyforVeterinary</t>
   </si>
   <si>
     <t>FeeOptimizerforVeterinary</t>
   </si>
   <si>
+    <t>VeterinaryPOPremium</t>
+  </si>
+  <si>
     <t>VeterinaryOCE</t>
   </si>
   <si>
-    <t>VeterinaryPOPremium</t>
-  </si>
-  <si>
-    <t>FeeSurveyforVeterinary</t>
-  </si>
-  <si>
     <t>SikkaSwellVetBundle</t>
   </si>
   <si>
+    <t>HillsToHome</t>
+  </si>
+  <si>
     <t>RoyalCanin</t>
   </si>
   <si>
-    <t>HillsToHome</t>
-  </si>
-  <si>
-    <t>Physician</t>
-  </si>
-  <si>
-    <t>Optometry</t>
-  </si>
-  <si>
-    <t>Chiropractic</t>
+    <t>physician</t>
+  </si>
+  <si>
+    <t>optometry</t>
+  </si>
+  <si>
+    <t>chiropractic</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s" s="20">
         <v>55</v>
@@ -759,7 +759,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s" s="20">
         <v>55</v>
@@ -773,7 +773,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s" s="20">
         <v>55</v>
@@ -787,7 +787,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s" s="20">
         <v>55</v>
@@ -867,7 +867,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s" s="24">
         <v>63</v>
@@ -881,7 +881,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s" s="24">
         <v>63</v>
@@ -895,7 +895,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s" s="24">
         <v>63</v>
@@ -909,7 +909,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s" s="24">
         <v>63</v>
@@ -956,7 +956,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s" s="26">
         <v>63</v>
@@ -1036,7 +1036,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s" s="30">
         <v>63</v>
@@ -1050,7 +1050,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s" s="30">
         <v>63</v>
@@ -1097,7 +1097,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s" s="32">
         <v>64</v>
@@ -1111,7 +1111,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="32">
         <v>64</v>
@@ -1158,7 +1158,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s" s="34">
         <v>64</v>
@@ -1172,7 +1172,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s" s="34">
         <v>64</v>
@@ -1186,7 +1186,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s" s="34">
         <v>64</v>
@@ -1200,7 +1200,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s" s="34">
         <v>64</v>
@@ -1275,7 +1275,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s" s="36">
         <v>64</v>
@@ -1322,7 +1322,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s" s="38">
         <v>64</v>
@@ -1612,7 +1612,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s" s="40">
         <v>64</v>
@@ -1640,7 +1640,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s" s="40">
         <v>64</v>
@@ -1687,7 +1687,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s" s="42">
         <v>65</v>
@@ -1701,7 +1701,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="42">
         <v>65</v>
@@ -1748,7 +1748,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s" s="44">
         <v>65</v>
@@ -1762,7 +1762,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s" s="44">
         <v>65</v>
@@ -1776,7 +1776,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s" s="44">
         <v>65</v>
@@ -1790,7 +1790,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s" s="44">
         <v>65</v>
@@ -1804,7 +1804,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s" s="44">
         <v>65</v>
@@ -1818,7 +1818,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s" s="44">
         <v>65</v>
@@ -1865,7 +1865,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s" s="46">
         <v>65</v>
@@ -1879,7 +1879,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s" s="46">
         <v>65</v>
@@ -1926,7 +1926,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s" s="48">
         <v>65</v>
@@ -1973,7 +1973,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s" s="50">
         <v>65</v>
@@ -2001,7 +2001,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s" s="50">
         <v>65</v>
@@ -2015,7 +2015,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s" s="50">
         <v>65</v>
@@ -2427,7 +2427,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s" s="12">
         <v>55</v>
@@ -2455,7 +2455,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s" s="12">
         <v>55</v>
@@ -2483,7 +2483,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s" s="12">
         <v>55</v>
@@ -2497,7 +2497,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s" s="12">
         <v>55</v>
@@ -2558,7 +2558,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s" s="14">
         <v>55</v>
@@ -2572,7 +2572,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s" s="14">
         <v>55</v>
@@ -2586,7 +2586,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s" s="14">
         <v>55</v>
@@ -2600,7 +2600,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s" s="14">
         <v>55</v>
@@ -2614,7 +2614,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s" s="14">
         <v>55</v>
@@ -2628,7 +2628,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s" s="14">
         <v>55</v>
@@ -2675,7 +2675,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s" s="16">
         <v>55</v>
@@ -2689,7 +2689,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s" s="16">
         <v>55</v>
@@ -2736,7 +2736,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s" s="18">
         <v>55</v>
@@ -2750,7 +2750,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s" s="18">
         <v>55</v>
@@ -2764,7 +2764,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s" s="18">
         <v>55</v>

</xml_diff>